<commit_message>
sessionize import and talk languages
</commit_message>
<xml_diff>
--- a/src/assets/speakers/data-advanced.xlsx
+++ b/src/assets/speakers/data-advanced.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="518">
   <si>
     <t>Session Id</t>
   </si>
@@ -76,44 +76,6 @@
   </si>
   <si>
     <t>Speaker Ids</t>
-  </si>
-  <si>
-    <t>More than Incognito: server-side secret searches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nowadays, privacy is a topic that comes up more and more often. Whenever you use a service or a platform, the provider typically knows exactly what you're doing and what you're interested in. But what if you don’t want the providers to know?_x000D_
-_x000D_
-In this talk, we'll explore a different perspective on privacy, specifically, the scenario where you want to access data from a public database without revealing what you're looking for. We’ll discuss how this can be done, along with the advantages and disadvantages of the various solutions available to achieve this kind of privacy.</t>
-  </si>
-  <si>
-    <t>Mariagiovanna Rotundo</t>
-  </si>
-  <si>
-    <t>mariagiovannarotundo@gmail.com</t>
-  </si>
-  <si>
-    <t>Cloud</t>
-  </si>
-  <si>
-    <t>Short (20min)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Introductory</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>f8ffd44d-f336-4c8c-baf7-b3ec73cfff60</t>
   </si>
   <si>
     <t>Breaking Free from the Need for Male Approval in Professional Growth</t>
@@ -143,6 +105,18 @@
     <t>Full (40min)</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>Introductory</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>united kingdom</t>
   </si>
   <si>
@@ -181,6 +155,9 @@
     <t>Yes, and I will be applying with Google's speaker program</t>
   </si>
   <si>
+    <t>Italy</t>
+  </si>
+  <si>
     <t>Sala Pacinotti</t>
   </si>
   <si>
@@ -200,7 +177,7 @@
     <t>gregoriopalama@gmail.com</t>
   </si>
   <si>
-    <t>Italian, English</t>
+    <t>Cloud</t>
   </si>
   <si>
     <t>Italia</t>
@@ -227,9 +204,6 @@
   </si>
   <si>
     <t>Mobile</t>
-  </si>
-  <si>
-    <t>English, Italian</t>
   </si>
   <si>
     <t>Sala Ricci</t>
@@ -329,7 +303,27 @@
     <t>jgiak92@gmail.com</t>
   </si>
   <si>
+    <t>Short (20min)</t>
+  </si>
+  <si>
     <t>a4b0383e-705e-4e23-9929-338c8e7783b0</t>
+  </si>
+  <si>
+    <t>More than Incognito: server-side secret searches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nowadays, privacy is a topic that comes up more and more often. Whenever you use a service or a platform, the provider typically knows exactly what you're doing and what you're interested in. But what if you don’t want the providers to know?_x000D_
+_x000D_
+In this talk, we'll explore a different perspective on privacy, specifically, the scenario where you want to access data from a public database without revealing what you're looking for. We’ll discuss how this can be done, along with the advantages and disadvantages of the various solutions available to achieve this kind of privacy.</t>
+  </si>
+  <si>
+    <t>Mariagiovanna Rotundo</t>
+  </si>
+  <si>
+    <t>mariagiovannarotundo@gmail.com</t>
+  </si>
+  <si>
+    <t>f8ffd44d-f336-4c8c-baf7-b3ec73cfff60</t>
   </si>
   <si>
     <t>Overlay and Arazzo: From API Definitions to API Experiences</t>
@@ -346,6 +340,9 @@
     <t>gloria.ciavarrini@gmail.com</t>
   </si>
   <si>
+    <t>English, Italian</t>
+  </si>
+  <si>
     <t>b1ee9ed2-fb20-4888-9d86-2835539d3528</t>
   </si>
   <si>
@@ -428,6 +425,77 @@
   </si>
   <si>
     <t>527b2a7b-fd99-4ba2-a076-5703226fbf03</t>
+  </si>
+  <si>
+    <t>Crafting Digital Twins with an Actor Model in Rust</t>
+  </si>
+  <si>
+    <t>Digital Twins represent a powerful paradigm for modelling complex IoT systems, yet practical implementations often fall short of theoretical promises. This talk cuts through the hype by demonstrating a robust approach based on an Actor Model pattern implemented in Rust, bridging the gap between conceptual frameworks and pragmatic engineering. Concurrency fundamentals, message-driven design patterns, and real-world use cases illustrate how Rust’s safety and performance guarantees enable maintainable, production-ready Digital Twin solutions.</t>
+  </si>
+  <si>
+    <t>Gianluca Insolvibile</t>
+  </si>
+  <si>
+    <t>g.insolvibile@nextworks.it</t>
+  </si>
+  <si>
+    <t>849b385a-5cc2-4a5e-a32e-b3e04c5ed10e</t>
+  </si>
+  <si>
+    <t>Personalizzare l'IA per il Diritto: Addestrare Modelli su Dataset Legali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’intelligenza artificiale può essere adattata per compiti specifici tramite il fine-tuning di modelli pre-addestrati, trasformandoli in strumenti altamente specializzati. In questo talk presenterò un progetto pratico basato su GPT-2, personalizzato per comprendere e generare testi giuridici, con un focus sull’interpretazione del Codice Civile e Penale e sulla creazione automatizzata di querele. Il progetto sfrutta tecnologie open source per ottimizzare un modello di linguaggio già esistente, rendendolo capace di rispondere a domande legali e generare documenti strutturati con un linguaggio formale e contestualizzato._x000D_
+Durante l’intervento illustrerò il workflow seguito, suddiviso in tre fasi principali. La prima riguarda la preparazione del dataset, che prevede l’estrazione dei testi normativi tramite web scraping e parsing, seguita dalla pulizia e tokenizzazione del testo con NLTK e Hugging Face Tokenizers, per garantire un’elaborazione efficace del linguaggio giuridico. La seconda fase si concentra sul fine-tuning di GPT-2, eseguito con PyTorch e TensorFlow per adattare il modello al dominio legale. Verranno ottimizzati iperparametri chiave come batch size, learning rate ed epoche, applicando tecniche di early stopping e gradient accumulation per migliorare le prestazioni su hardware limitato. Infine, nella terza fase, verrà presentata l’interfaccia web, sviluppata con Flask, che consente agli utenti di inserire domande giuridiche o descrivere un caso, ricevendo in risposta un’analisi legale dettagliata o una bozza di querela generata automaticamente dal modello._x000D_
+Il talk si concluderà con una demo live, dimostrando come la personalizzazione di GPT-2 possa trasformare un modello generico in uno strumento avanzato per il settore giuridico. L'obiettivo è mostrare come sia possibile adattare un LLM alle esigenze specifiche di qualsiasi organizzazione o settore.</t>
+  </si>
+  <si>
+    <t>Daniele Mario Areddu</t>
+  </si>
+  <si>
+    <t>danielemario@areddu.it</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>919f1380-f9b7-40ce-97a9-545be75734ae</t>
+  </si>
+  <si>
+    <t>How to give your first Talk without freaking out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public speaking can be intimidating: where do we start from? How to find the right topic? How to put together a nice presentation? Will the audience ask me questions? In this talk I will provide first hand tips I learned the hard way on how to go from zero to give your first public talk with confidence._x000D_
+</t>
+  </si>
+  <si>
+    <t>Federico Paolinelli</t>
+  </si>
+  <si>
+    <t>fedepaol@gmail.com</t>
+  </si>
+  <si>
+    <t>d26a7c22-25fc-466d-89ff-c0a77c93f820</t>
+  </si>
+  <si>
+    <t>Beats in the Browser - Coding Music with JavaScript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javascript is extremely versatile. We use it to build frontend, backend, desktop and mobile apps. But did you know you can even create music with it ?!_x000D_
+_x000D_
+In this talk, Rowdy will show you how easy and fun it is to code your own music with the Web Audio API. As a bonus, he will throw in the Web MIDI API and Web Bluetooth API to really get the party started. Let’s turn up the bass!</t>
+  </si>
+  <si>
+    <t>Rowdy Rabouw</t>
+  </si>
+  <si>
+    <t>hi@rowdy.codes</t>
+  </si>
+  <si>
+    <t>The Netherlands</t>
+  </si>
+  <si>
+    <t>f5c30de4-cd93-4022-97f6-b0a58c92197c</t>
   </si>
   <si>
     <t>La Musica Del Malware</t>
@@ -449,57 +517,6 @@
   </si>
   <si>
     <t>96c13f58-033e-4f7a-8401-edcc8370009b, 3d9a3287-cc36-4428-b6b4-1dd1df1e70e8</t>
-  </si>
-  <si>
-    <t>Crafting Digital Twins with an Actor Model in Rust</t>
-  </si>
-  <si>
-    <t>Digital Twins represent a powerful paradigm for modelling complex IoT systems, yet practical implementations often fall short of theoretical promises. This talk cuts through the hype by demonstrating a robust approach based on an Actor Model pattern implemented in Rust, bridging the gap between conceptual frameworks and pragmatic engineering. Concurrency fundamentals, message-driven design patterns, and real-world use cases illustrate how Rust’s safety and performance guarantees enable maintainable, production-ready Digital Twin solutions.</t>
-  </si>
-  <si>
-    <t>Gianluca Insolvibile</t>
-  </si>
-  <si>
-    <t>g.insolvibile@nextworks.it</t>
-  </si>
-  <si>
-    <t>849b385a-5cc2-4a5e-a32e-b3e04c5ed10e</t>
-  </si>
-  <si>
-    <t>How to give your first Talk without freaking out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Public speaking can be intimidating: where do we start from? How to find the right topic? How to put together a nice presentation? Will the audience ask me questions? In this talk I will provide first hand tips I learned the hard way on how to go from zero to give your first public talk with confidence._x000D_
-</t>
-  </si>
-  <si>
-    <t>Federico Paolinelli</t>
-  </si>
-  <si>
-    <t>fedepaol@gmail.com</t>
-  </si>
-  <si>
-    <t>d26a7c22-25fc-466d-89ff-c0a77c93f820</t>
-  </si>
-  <si>
-    <t>Beats in the Browser - Coding Music with JavaScript</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javascript is extremely versatile. We use it to build frontend, backend, desktop and mobile apps. But did you know you can even create music with it ?!_x000D_
-_x000D_
-In this talk, Rowdy will show you how easy and fun it is to code your own music with the Web Audio API. As a bonus, he will throw in the Web MIDI API and Web Bluetooth API to really get the party started. Let’s turn up the bass!</t>
-  </si>
-  <si>
-    <t>Rowdy Rabouw</t>
-  </si>
-  <si>
-    <t>hi@rowdy.codes</t>
-  </si>
-  <si>
-    <t>The Netherlands</t>
-  </si>
-  <si>
-    <t>f5c30de4-cd93-4022-97f6-b0a58c92197c</t>
   </si>
   <si>
     <t>Sailing the Waters using UI/UX Reinforced by Security</t>
@@ -539,63 +556,6 @@
     <t>493590fc-c38a-4f7f-b76f-e81d7cf6207a</t>
   </si>
   <si>
-    <t>Personalizzare l'IA per il Diritto: Addestrare Modelli su Dataset Legali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’intelligenza artificiale può essere adattata per compiti specifici tramite il fine-tuning di modelli pre-addestrati, trasformandoli in strumenti altamente specializzati. In questo talk presenterò un progetto pratico basato su GPT-2, personalizzato per comprendere e generare testi giuridici, con un focus sull’interpretazione del Codice Civile e Penale e sulla creazione automatizzata di querele. Il progetto sfrutta tecnologie open source per ottimizzare un modello di linguaggio già esistente, rendendolo capace di rispondere a domande legali e generare documenti strutturati con un linguaggio formale e contestualizzato._x000D_
-Durante l’intervento illustrerò il workflow seguito, suddiviso in tre fasi principali. La prima riguarda la preparazione del dataset, che prevede l’estrazione dei testi normativi tramite web scraping e parsing, seguita dalla pulizia e tokenizzazione del testo con NLTK e Hugging Face Tokenizers, per garantire un’elaborazione efficace del linguaggio giuridico. La seconda fase si concentra sul fine-tuning di GPT-2, eseguito con PyTorch e TensorFlow per adattare il modello al dominio legale. Verranno ottimizzati iperparametri chiave come batch size, learning rate ed epoche, applicando tecniche di early stopping e gradient accumulation per migliorare le prestazioni su hardware limitato. Infine, nella terza fase, verrà presentata l’interfaccia web, sviluppata con Flask, che consente agli utenti di inserire domande giuridiche o descrivere un caso, ricevendo in risposta un’analisi legale dettagliata o una bozza di querela generata automaticamente dal modello._x000D_
-Il talk si concluderà con una demo live, dimostrando come la personalizzazione di GPT-2 possa trasformare un modello generico in uno strumento avanzato per il settore giuridico. L'obiettivo è mostrare come sia possibile adattare un LLM alle esigenze specifiche di qualsiasi organizzazione o settore.</t>
-  </si>
-  <si>
-    <t>Daniele Mario Areddu</t>
-  </si>
-  <si>
-    <t>danielemario@areddu.it</t>
-  </si>
-  <si>
-    <t>Advanced</t>
-  </si>
-  <si>
-    <t>919f1380-f9b7-40ce-97a9-545be75734ae</t>
-  </si>
-  <si>
-    <t>Extending Kubernetes: Building torproxy for Anonymous Container Communication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">torproxy is an open source Kubernetes controller written in Go to enable tor utilities in your k8s cluster. _x000D_
-We will go through the implementation of a generic controller, taking as example the torproxy._x000D_
-The audience will learn more about writing kubernetes controllers, know more about tor network, Go language patterns </t>
-  </si>
-  <si>
-    <t>Fulvio Denza</t>
-  </si>
-  <si>
-    <t>fulviodenza823@gmail.com</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>fc2a3a72-76e2-4a5d-b05b-cf02838714e5</t>
-  </si>
-  <si>
-    <t>Form inclusivi: l'importanza dei dettagli nascosti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I form sono spesso la porta d'ingresso ai servizi online. Come possiamo renderli più inclusivi per gli utenti?_x000D_
-Progettare e sviluppare un form inclusivo richiede una serie di considerazioni da fare nelle varie fasi del processo di realizzazione, che spesso vengono ignorate o date per scontate._x000D_
-Scopriamo insieme come ridefinire un form e renderlo più inclusivo.</t>
-  </si>
-  <si>
-    <t>Loredana Frontino</t>
-  </si>
-  <si>
-    <t>lory.frontino@gmail.com</t>
-  </si>
-  <si>
-    <t>71dba3f8-a0f9-4301-a3a7-d699aa1a182b</t>
-  </si>
-  <si>
     <t>Boost your LLM-based application with a RAG system</t>
   </si>
   <si>
@@ -613,6 +573,23 @@
   </si>
   <si>
     <t>23778c1e-25bf-477e-b1bd-a577b88a1205</t>
+  </si>
+  <si>
+    <t>Form inclusivi: l'importanza dei dettagli nascosti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I form sono spesso la porta d'ingresso ai servizi online. Come possiamo renderli più inclusivi per gli utenti?_x000D_
+Progettare e sviluppare un form inclusivo richiede una serie di considerazioni da fare nelle varie fasi del processo di realizzazione, che spesso vengono ignorate o date per scontate._x000D_
+Scopriamo insieme come ridefinire un form e renderlo più inclusivo.</t>
+  </si>
+  <si>
+    <t>Loredana Frontino</t>
+  </si>
+  <si>
+    <t>lory.frontino@gmail.com</t>
+  </si>
+  <si>
+    <t>71dba3f8-a0f9-4301-a3a7-d699aa1a182b</t>
   </si>
   <si>
     <t>Verso una logistica intelligente: AI e Apprendimento Federato per ottimizzare processi logistici</t>
@@ -633,6 +610,26 @@
   </si>
   <si>
     <t>cdc81ad6-0f52-4e99-87b3-a95ab9863b1a</t>
+  </si>
+  <si>
+    <t>Extending Kubernetes: Building torproxy for Anonymous Container Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">torproxy is an open source Kubernetes controller written in Go to enable tor utilities in your k8s cluster. _x000D_
+We will go through the implementation of a generic controller, taking as example the torproxy._x000D_
+The audience will learn more about writing kubernetes controllers, know more about tor network, Go language patterns </t>
+  </si>
+  <si>
+    <t>Fulvio Denza</t>
+  </si>
+  <si>
+    <t>fulviodenza823@gmail.com</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>fc2a3a72-76e2-4a5d-b05b-cf02838714e5</t>
   </si>
   <si>
     <t>How I ported Doom to the browser with WebAssembly</t>
@@ -723,7 +720,7 @@
     <t>8730d40b-3fb7-450d-ab71-08c9dd81a48a</t>
   </si>
   <si>
-    <t>Addestra il tuo LLM a pensare con GRPO—ora anche su piccole GPU!</t>
+    <t>Addestra il tuo LLM a pensare con GRPO — ora anche su piccole GPU!</t>
   </si>
   <si>
     <t xml:space="preserve">DeepSeek R1, uno dei large language model più discussi del momento, ha introdotto GRPO, un nuovo algoritmo di reinforcement learning che permetterebbe di addestrare modelli che "ragionano". Ma è davvero così?_x000D_
@@ -1853,7 +1850,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>854505</v>
+        <v>850062</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>21</v>
@@ -1891,161 +1888,167 @@
       <c r="M2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>30</v>
+      <c r="N2" s="5">
+        <v>45714.409613923606</v>
+      </c>
+      <c r="O2" s="5">
+        <v>45720.697022025459</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>45759.416666666664</v>
+      </c>
+      <c r="R2" s="0">
+        <v>45</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>850062</v>
+        <v>860330</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N3" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O3" s="5">
-        <v>45720.697022025459</v>
+        <v>45715.323366666664</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="5">
         <v>45759.416666666664</v>
       </c>
       <c r="R3" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>860330</v>
+        <v>862668</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="N4" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O4" s="5">
-        <v>45715.323366666664</v>
+        <v>45730.456549537033</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="5">
         <v>45759.416666666664</v>
       </c>
       <c r="R4" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>862668</v>
+        <v>862926</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="G5" s="0" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>27</v>
@@ -2054,19 +2057,19 @@
         <v>28</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="N5" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O5" s="5">
-        <v>45730.456549537033</v>
+        <v>45714.860351701383</v>
       </c>
       <c r="P5" s="0" t="s">
         <v>58</v>
@@ -2075,7 +2078,7 @@
         <v>45759.416666666664</v>
       </c>
       <c r="R5" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U5" s="0" t="s">
         <v>59</v>
@@ -2083,7 +2086,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>862926</v>
+        <v>797393</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>60</v>
@@ -2101,10 +2104,10 @@
         <v>62</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>27</v>
@@ -2113,57 +2116,57 @@
         <v>28</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N6" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O6" s="5">
-        <v>45714.860351701383</v>
+        <v>45714.416337303242</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q6" s="5">
-        <v>45759.416666666664</v>
+        <v>45759.451388888891</v>
       </c>
       <c r="R6" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>797393</v>
+        <v>821974</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>27</v>
@@ -2172,57 +2175,57 @@
         <v>28</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N7" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O7" s="5">
-        <v>45714.416337303242</v>
+        <v>45714.488690428239</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="Q7" s="5">
         <v>45759.451388888891</v>
       </c>
       <c r="R7" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>821974</v>
+        <v>838947</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="F8" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="H8" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>27</v>
@@ -2231,175 +2234,175 @@
         <v>28</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N8" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O8" s="5">
-        <v>45714.488690428239</v>
+        <v>45714.437480636574</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="Q8" s="5">
         <v>45759.451388888891</v>
       </c>
       <c r="R8" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>838947</v>
+        <v>862301</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>81</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>80</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N9" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O9" s="5">
-        <v>45714.437480636574</v>
+        <v>45714.446214780088</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="Q9" s="5">
         <v>45759.451388888891</v>
       </c>
       <c r="R9" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>862301</v>
+        <v>796625</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="E10" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N10" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O10" s="5">
-        <v>45714.446214780088</v>
+        <v>45714.444721261571</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="5">
-        <v>45759.451388888891</v>
+        <v>45759.486111111109</v>
       </c>
       <c r="R10" s="0">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>796625</v>
+        <v>854505</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="F11" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>27</v>
@@ -2408,31 +2411,31 @@
         <v>28</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="N11" s="5">
-        <v>45714.409613923606</v>
-      </c>
-      <c r="O11" s="5">
-        <v>45714.444721261571</v>
+        <v>42</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="Q11" s="5">
         <v>45759.486111111109</v>
       </c>
       <c r="R11" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12">
@@ -2440,25 +2443,25 @@
         <v>860892</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="E12" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="F12" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>27</v>
@@ -2467,13 +2470,13 @@
         <v>28</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N12" s="5">
         <v>45714.409613923606</v>
@@ -2482,16 +2485,16 @@
         <v>45714.545749652774</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="5">
         <v>45759.486111111109</v>
       </c>
       <c r="R12" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13">
@@ -2499,40 +2502,40 @@
         <v>883240</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>104</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="N13" s="0" t="s">
         <v>30</v>
@@ -2541,16 +2544,16 @@
         <v>30</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="Q13" s="5">
         <v>45759.486111111109</v>
       </c>
       <c r="R13" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14">
@@ -2558,25 +2561,25 @@
         <v>824924</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>27</v>
@@ -2585,13 +2588,13 @@
         <v>28</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N14" s="5">
         <v>45714.409613923606</v>
@@ -2600,16 +2603,16 @@
         <v>45715.407090312496</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="Q14" s="5">
         <v>45759.506944444445</v>
       </c>
       <c r="R14" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15">
@@ -2617,25 +2620,25 @@
         <v>859518</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="E15" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>114</v>
-      </c>
       <c r="F15" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>27</v>
@@ -2644,13 +2647,13 @@
         <v>28</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N15" s="5">
         <v>45714.409613923606</v>
@@ -2659,16 +2662,16 @@
         <v>45714.440862071759</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="Q15" s="5">
         <v>45759.506944444445</v>
       </c>
       <c r="R15" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16">
@@ -2676,40 +2679,40 @@
         <v>859594</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="D16" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>120</v>
-      </c>
       <c r="G16" s="0" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N16" s="5">
         <v>45714.409613923606</v>
@@ -2718,16 +2721,16 @@
         <v>45714.5267258449</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q16" s="5">
         <v>45759.506944444445</v>
       </c>
       <c r="R16" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17">
@@ -2735,40 +2738,40 @@
         <v>884731</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>125</v>
-      </c>
       <c r="F17" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N17" s="0" t="s">
         <v>30</v>
@@ -2777,134 +2780,134 @@
         <v>30</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="Q17" s="5">
         <v>45759.506944444445</v>
       </c>
       <c r="R17" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>822693</v>
+        <v>846889</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="F18" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="N18" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O18" s="5">
-        <v>45715.34785543981</v>
+        <v>45714.435481863424</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q18" s="5">
         <v>45759.583333333328</v>
       </c>
       <c r="R18" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>846889</v>
+        <v>853115</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="E19" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>136</v>
-      </c>
       <c r="F19" s="0" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N19" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O19" s="5">
-        <v>45714.435481863424</v>
+        <v>45714.418413229163</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="Q19" s="5">
         <v>45759.583333333328</v>
       </c>
       <c r="R19" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20">
@@ -2912,25 +2915,25 @@
         <v>857773</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="E20" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>141</v>
-      </c>
       <c r="F20" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>27</v>
@@ -2945,7 +2948,7 @@
         <v>30</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N20" s="5">
         <v>45714.409613923606</v>
@@ -2954,16 +2957,16 @@
         <v>45714.595782326389</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="Q20" s="5">
         <v>45759.583333333328</v>
       </c>
       <c r="R20" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U20" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21">
@@ -2971,40 +2974,40 @@
         <v>857916</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>146</v>
-      </c>
       <c r="F21" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K21" s="0" t="s">
         <v>29</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N21" s="5">
         <v>45714.409613923606</v>
@@ -3013,101 +3016,101 @@
         <v>45714.4301599537</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q21" s="5">
         <v>45759.583333333328</v>
       </c>
       <c r="R21" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U21" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>837938</v>
+        <v>822693</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="F22" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="F22" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="G22" s="0" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>153</v>
+        <v>50</v>
       </c>
       <c r="N22" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O22" s="5">
-        <v>45714.433191932869</v>
+        <v>45715.34785543981</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="Q22" s="5">
         <v>45759.618055555555</v>
       </c>
       <c r="R22" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U22" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>843163</v>
+        <v>837938</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="E23" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="F23" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>27</v>
@@ -3116,28 +3119,28 @@
         <v>28</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="N23" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O23" s="5">
-        <v>45714.551208599536</v>
+        <v>45714.433191932869</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="Q23" s="5">
         <v>45759.618055555555</v>
       </c>
       <c r="R23" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U23" s="0" t="s">
         <v>159</v>
@@ -3145,7 +3148,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>853115</v>
+        <v>843163</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>160</v>
@@ -3163,75 +3166,75 @@
         <v>162</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>164</v>
+        <v>28</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L24" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="N24" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O24" s="5">
-        <v>45714.418413229163</v>
+        <v>45714.551208599536</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="Q24" s="5">
         <v>45759.618055555555</v>
       </c>
       <c r="R24" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U24" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>863474</v>
+        <v>849512</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>169</v>
-      </c>
       <c r="F25" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>29</v>
@@ -3240,25 +3243,25 @@
         <v>30</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="N25" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O25" s="5">
-        <v>45714.481459178241</v>
+        <v>45714.431661076385</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="Q25" s="5">
         <v>45759.618055555555</v>
       </c>
       <c r="R25" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U25" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26">
@@ -3266,25 +3269,25 @@
         <v>813458</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="E26" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>175</v>
-      </c>
       <c r="F26" s="0" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>27</v>
@@ -3293,13 +3296,13 @@
         <v>28</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N26" s="5">
         <v>45714.409613923606</v>
@@ -3308,7 +3311,7 @@
         <v>45714.436776504626</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="Q26" s="5">
         <v>45759.652777777774</v>
@@ -3317,89 +3320,89 @@
         <v>25</v>
       </c>
       <c r="U26" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>849512</v>
+        <v>863339</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="E27" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>180</v>
-      </c>
       <c r="F27" s="0" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="I27" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="L27" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="N27" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O27" s="5">
-        <v>45714.431661076385</v>
+        <v>45716.368220023149</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="Q27" s="5">
         <v>45759.652777777774</v>
       </c>
       <c r="R27" s="0">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="U27" s="0" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>863339</v>
+        <v>863474</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="E28" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>185</v>
-      </c>
       <c r="F28" s="0" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>26</v>
@@ -3408,34 +3411,34 @@
         <v>27</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="L28" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>57</v>
+        <v>184</v>
       </c>
       <c r="N28" s="5">
         <v>45714.409613923606</v>
       </c>
       <c r="O28" s="5">
-        <v>45716.368220023149</v>
+        <v>45714.481459178241</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q28" s="5">
         <v>45759.652777777774</v>
       </c>
       <c r="R28" s="0">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="U28" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29">
@@ -3443,31 +3446,31 @@
         <v>863806</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="D29" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="E29" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="E29" s="0" t="s">
-        <v>190</v>
-      </c>
       <c r="F29" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K29" s="0" t="s">
         <v>29</v>
@@ -3476,7 +3479,7 @@
         <v>30</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N29" s="5">
         <v>45714.409613923606</v>
@@ -3485,16 +3488,16 @@
         <v>45714.463723611108</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q29" s="5">
         <v>45759.652777777774</v>
       </c>
       <c r="R29" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U29" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30">
@@ -3502,25 +3505,25 @@
         <v>862602</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>196</v>
-      </c>
       <c r="F30" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>27</v>
@@ -3529,13 +3532,13 @@
         <v>28</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L30" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N30" s="5">
         <v>45714.409613923606</v>
@@ -3544,7 +3547,7 @@
         <v>45714.425511076384</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="Q30" s="5">
         <v>45759.670138888891</v>
@@ -3553,7 +3556,7 @@
         <v>25</v>
       </c>
       <c r="U30" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31">
@@ -3561,25 +3564,25 @@
         <v>885792</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="E31" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="E31" s="0" t="s">
-        <v>201</v>
-      </c>
       <c r="F31" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>27</v>
@@ -3588,13 +3591,13 @@
         <v>28</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="L31" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N31" s="0" t="s">
         <v>30</v>
@@ -3603,7 +3606,7 @@
         <v>30</v>
       </c>
       <c r="P31" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="Q31" s="5">
         <v>45759.670138888891</v>
@@ -3612,7 +3615,7 @@
         <v>25</v>
       </c>
       <c r="U31" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32">
@@ -3620,25 +3623,25 @@
         <v>857452</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="D32" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="E32" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>206</v>
-      </c>
       <c r="F32" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>27</v>
@@ -3650,10 +3653,10 @@
         <v>29</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="M32" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N32" s="5">
         <v>45695.507444594907</v>
@@ -3662,16 +3665,16 @@
         <v>45695.538855474537</v>
       </c>
       <c r="P32" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q32" s="5">
         <v>45759.708333333328</v>
       </c>
       <c r="R32" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U32" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33">
@@ -3679,40 +3682,40 @@
         <v>861129</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="D33" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="E33" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>212</v>
-      </c>
       <c r="F33" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I33" s="0" t="s">
         <v>27</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="L33" s="0" t="s">
         <v>27</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N33" s="0" t="s">
         <v>30</v>
@@ -3721,16 +3724,16 @@
         <v>30</v>
       </c>
       <c r="P33" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="Q33" s="5">
         <v>45759.708333333328</v>
       </c>
       <c r="R33" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U33" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34">
@@ -3738,25 +3741,25 @@
         <v>864118</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="D34" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="E34" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>217</v>
-      </c>
       <c r="F34" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>27</v>
@@ -3771,7 +3774,7 @@
         <v>30</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N34" s="5">
         <v>45714.409613923606</v>
@@ -3780,16 +3783,16 @@
         <v>45714.806715277773</v>
       </c>
       <c r="P34" s="0" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="Q34" s="5">
         <v>45759.708333333328</v>
       </c>
       <c r="R34" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U34" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35">
@@ -3797,25 +3800,25 @@
         <v>893277</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="D35" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="E35" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>222</v>
-      </c>
       <c r="F35" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>27</v>
@@ -3830,7 +3833,7 @@
         <v>30</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N35" s="0" t="s">
         <v>30</v>
@@ -3839,16 +3842,16 @@
         <v>30</v>
       </c>
       <c r="P35" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="Q35" s="5">
         <v>45759.708333333328</v>
       </c>
       <c r="R35" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U35" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36">
@@ -3856,25 +3859,25 @@
         <v>826068</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="D36" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="E36" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="E36" s="0" t="s">
-        <v>227</v>
-      </c>
       <c r="F36" s="0" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>27</v>
@@ -3883,13 +3886,13 @@
         <v>28</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="L36" s="0" t="s">
         <v>30</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="N36" s="5">
         <v>45714.409613923606</v>
@@ -3898,16 +3901,16 @@
         <v>45714.422330590278</v>
       </c>
       <c r="P36" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="Q36" s="5">
         <v>45759.743055555555</v>
       </c>
       <c r="R36" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="U36" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3925,1173 +3928,1173 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>248</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>257</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>266</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="M5" s="0" t="s">
         <v>273</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="M6" s="0" t="s">
         <v>281</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="H7" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="M7" s="0" t="s">
         <v>287</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="M8" s="0" t="s">
         <v>292</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="I9" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="M9" s="0" t="s">
         <v>300</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="G10" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="J10" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="M10" s="0" t="s">
         <v>307</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="M11" s="0" t="s">
         <v>313</v>
-      </c>
-      <c r="M11" s="0" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="M12" s="0" t="s">
         <v>318</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="I13" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="J13" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="K13" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="M13" s="0" t="s">
         <v>328</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>331</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="L14" s="0" t="s">
         <v>335</v>
       </c>
-      <c r="L14" s="0" t="s">
+      <c r="M14" s="0" t="s">
         <v>336</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="C15" s="0" t="s">
         <v>339</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="G15" s="0" t="s">
         <v>341</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="H15" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="M15" s="0" t="s">
         <v>342</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="M15" s="0" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>344</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="D16" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>345</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="G16" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="M16" s="0" t="s">
         <v>348</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="M17" s="0" t="s">
         <v>354</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="E18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>358</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="G18" s="0" t="s">
         <v>359</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="M18" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="D19" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="F19" s="0" t="s">
         <v>364</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="G19" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="H19" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="J19" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="J19" s="0" t="s">
+      <c r="K19" s="0" t="s">
         <v>368</v>
       </c>
-      <c r="K19" s="0" t="s">
+      <c r="M19" s="0" t="s">
         <v>369</v>
-      </c>
-      <c r="M19" s="0" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="F20" s="0" t="s">
         <v>373</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="G20" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="H20" s="0" t="s">
         <v>375</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="J20" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="K20" s="0" t="s">
         <v>377</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="M20" s="0" t="s">
         <v>378</v>
-      </c>
-      <c r="M20" s="0" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="F21" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="G21" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="H21" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="I21" s="0" t="s">
         <v>385</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="K21" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="M21" s="0" t="s">
         <v>387</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="F22" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="G22" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="I22" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="K22" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="M22" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>398</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="F23" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="I23" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="M23" s="0" t="s">
         <v>402</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>405</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="F24" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="G24" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="H24" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="I24" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="M24" s="0" t="s">
         <v>410</v>
-      </c>
-      <c r="M24" s="0" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="G25" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="K25" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="K25" s="0" t="s">
+      <c r="M25" s="0" t="s">
         <v>417</v>
-      </c>
-      <c r="M25" s="0" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="D26" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="F26" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="G26" s="0" t="s">
         <v>422</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="I26" s="0" t="s">
         <v>423</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="K26" s="0" t="s">
         <v>424</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="L26" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="L26" s="0" t="s">
+      <c r="M26" s="0" t="s">
         <v>426</v>
-      </c>
-      <c r="M26" s="0" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>428</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="D27" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>429</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="F27" s="0" t="s">
         <v>430</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="G27" s="0" t="s">
         <v>431</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="M27" s="0" t="s">
         <v>432</v>
-      </c>
-      <c r="M27" s="0" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>434</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="D28" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="F28" s="0" t="s">
         <v>436</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="G28" s="0" t="s">
         <v>437</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="H28" s="0" t="s">
         <v>438</v>
       </c>
-      <c r="H28" s="0" t="s">
+      <c r="I28" s="0" t="s">
         <v>439</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="K28" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="L28" s="0" t="s">
         <v>441</v>
       </c>
-      <c r="L28" s="0" t="s">
+      <c r="M28" s="0" t="s">
         <v>442</v>
-      </c>
-      <c r="M28" s="0" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="D29" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="0" t="s">
+      <c r="F29" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="G29" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="H29" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="I29" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="K29" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="L29" s="0" t="s">
         <v>451</v>
       </c>
-      <c r="L29" s="0" t="s">
+      <c r="M29" s="0" t="s">
         <v>452</v>
-      </c>
-      <c r="M29" s="0" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>455</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="F30" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="G30" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="J30" s="0" t="s">
         <v>458</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="M30" s="0" t="s">
         <v>459</v>
-      </c>
-      <c r="M30" s="0" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>461</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="C31" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>463</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="E31" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="F31" s="0" t="s">
         <v>465</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="G31" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="H31" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="M31" s="0" t="s">
         <v>467</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="M31" s="0" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>469</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="F32" s="0" t="s">
         <v>470</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="G32" s="0" t="s">
         <v>471</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="K32" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="K32" s="0" t="s">
+      <c r="M32" s="0" t="s">
         <v>473</v>
-      </c>
-      <c r="M32" s="0" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="D33" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="E33" s="0" t="s">
+      <c r="F33" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="G33" s="0" t="s">
         <v>478</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="H33" s="0" t="s">
         <v>479</v>
       </c>
-      <c r="H33" s="0" t="s">
+      <c r="I33" s="0" t="s">
         <v>480</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="M33" s="0" t="s">
         <v>481</v>
-      </c>
-      <c r="M33" s="0" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>483</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="F34" s="0" t="s">
         <v>484</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="G34" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="H34" s="0" t="s">
         <v>486</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="K34" s="0" t="s">
         <v>487</v>
       </c>
-      <c r="K34" s="0" t="s">
+      <c r="M34" s="0" t="s">
         <v>488</v>
-      </c>
-      <c r="M34" s="0" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>490</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="D35" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>491</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="F35" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="G35" s="0" t="s">
         <v>493</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="M35" s="0" t="s">
         <v>494</v>
-      </c>
-      <c r="M35" s="0" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>496</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="D36" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>497</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="F36" s="0" t="s">
         <v>498</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="G36" s="0" t="s">
         <v>499</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="H36" s="0" t="s">
         <v>500</v>
       </c>
-      <c r="H36" s="0" t="s">
+      <c r="I36" s="0" t="s">
         <v>501</v>
       </c>
-      <c r="I36" s="0" t="s">
+      <c r="J36" s="0" t="s">
         <v>502</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="K36" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="L36" s="0" t="s">
         <v>503</v>
       </c>
-      <c r="K36" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="L36" s="0" t="s">
+      <c r="M36" s="0" t="s">
         <v>504</v>
-      </c>
-      <c r="M36" s="0" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>506</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="D37" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="F37" s="0" t="s">
         <v>508</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="G37" s="0" t="s">
         <v>509</v>
       </c>
-      <c r="G37" s="0" t="s">
+      <c r="M37" s="0" t="s">
         <v>510</v>
-      </c>
-      <c r="M37" s="0" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>512</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="D38" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>513</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="F38" s="0" t="s">
         <v>514</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="G38" s="0" t="s">
         <v>515</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="H38" s="0" t="s">
         <v>516</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="M38" s="0" t="s">
         <v>517</v>
-      </c>
-      <c r="M38" s="0" t="s">
-        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated talk schedule and lang info
</commit_message>
<xml_diff>
--- a/src/assets/speakers/data-advanced.xlsx
+++ b/src/assets/speakers/data-advanced.xlsx
@@ -1901,7 +1901,7 @@
         <v>45759.416666666664</v>
       </c>
       <c r="R2" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U2" s="0" t="s">
         <v>33</v>
@@ -1960,7 +1960,7 @@
         <v>45759.416666666664</v>
       </c>
       <c r="R3" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U3" s="0" t="s">
         <v>44</v>
@@ -2019,7 +2019,7 @@
         <v>45759.416666666664</v>
       </c>
       <c r="R4" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U4" s="0" t="s">
         <v>52</v>
@@ -2078,7 +2078,7 @@
         <v>45759.416666666664</v>
       </c>
       <c r="R5" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U5" s="0" t="s">
         <v>59</v>
@@ -2137,7 +2137,7 @@
         <v>45759.451388888891</v>
       </c>
       <c r="R6" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>64</v>
@@ -2196,7 +2196,7 @@
         <v>45759.451388888891</v>
       </c>
       <c r="R7" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>69</v>
@@ -2255,7 +2255,7 @@
         <v>45759.451388888891</v>
       </c>
       <c r="R8" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>75</v>
@@ -2314,7 +2314,7 @@
         <v>45759.451388888891</v>
       </c>
       <c r="R9" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U9" s="0" t="s">
         <v>82</v>
@@ -2373,7 +2373,7 @@
         <v>45759.486111111109</v>
       </c>
       <c r="R10" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U10" s="0" t="s">
         <v>88</v>
@@ -2432,7 +2432,7 @@
         <v>45759.486111111109</v>
       </c>
       <c r="R11" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U11" s="0" t="s">
         <v>93</v>
@@ -2491,7 +2491,7 @@
         <v>45759.486111111109</v>
       </c>
       <c r="R12" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U12" s="0" t="s">
         <v>99</v>
@@ -2550,7 +2550,7 @@
         <v>45759.486111111109</v>
       </c>
       <c r="R13" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U13" s="0" t="s">
         <v>104</v>
@@ -2609,7 +2609,7 @@
         <v>45759.506944444445</v>
       </c>
       <c r="R14" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U14" s="0" t="s">
         <v>109</v>
@@ -2668,7 +2668,7 @@
         <v>45759.506944444445</v>
       </c>
       <c r="R15" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U15" s="0" t="s">
         <v>114</v>
@@ -2727,7 +2727,7 @@
         <v>45759.506944444445</v>
       </c>
       <c r="R16" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U16" s="0" t="s">
         <v>120</v>
@@ -2786,7 +2786,7 @@
         <v>45759.506944444445</v>
       </c>
       <c r="R17" s="0">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U17" s="0" t="s">
         <v>125</v>
@@ -2845,7 +2845,7 @@
         <v>45759.583333333328</v>
       </c>
       <c r="R18" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U18" s="0" t="s">
         <v>130</v>
@@ -2904,7 +2904,7 @@
         <v>45759.583333333328</v>
       </c>
       <c r="R19" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U19" s="0" t="s">
         <v>136</v>
@@ -2963,7 +2963,7 @@
         <v>45759.583333333328</v>
       </c>
       <c r="R20" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U20" s="0" t="s">
         <v>141</v>
@@ -3022,7 +3022,7 @@
         <v>45759.583333333328</v>
       </c>
       <c r="R21" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U21" s="0" t="s">
         <v>147</v>
@@ -3081,7 +3081,7 @@
         <v>45759.618055555555</v>
       </c>
       <c r="R22" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U22" s="0" t="s">
         <v>153</v>
@@ -3140,7 +3140,7 @@
         <v>45759.618055555555</v>
       </c>
       <c r="R23" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U23" s="0" t="s">
         <v>159</v>
@@ -3199,7 +3199,7 @@
         <v>45759.618055555555</v>
       </c>
       <c r="R24" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U24" s="0" t="s">
         <v>164</v>
@@ -3258,7 +3258,7 @@
         <v>45759.618055555555</v>
       </c>
       <c r="R25" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U25" s="0" t="s">
         <v>169</v>
@@ -3435,7 +3435,7 @@
         <v>45759.652777777774</v>
       </c>
       <c r="R28" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U28" s="0" t="s">
         <v>185</v>
@@ -3494,7 +3494,7 @@
         <v>45759.652777777774</v>
       </c>
       <c r="R29" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U29" s="0" t="s">
         <v>191</v>
@@ -3671,7 +3671,7 @@
         <v>45759.708333333328</v>
       </c>
       <c r="R32" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U32" s="0" t="s">
         <v>207</v>
@@ -3730,7 +3730,7 @@
         <v>45759.708333333328</v>
       </c>
       <c r="R33" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U33" s="0" t="s">
         <v>212</v>
@@ -3789,7 +3789,7 @@
         <v>45759.708333333328</v>
       </c>
       <c r="R34" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U34" s="0" t="s">
         <v>217</v>
@@ -3848,7 +3848,7 @@
         <v>45759.708333333328</v>
       </c>
       <c r="R35" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U35" s="0" t="s">
         <v>222</v>
@@ -3907,7 +3907,7 @@
         <v>45759.743055555555</v>
       </c>
       <c r="R36" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="U36" s="0" t="s">
         <v>227</v>

</xml_diff>